<commit_message>
fixes to example diary
</commit_message>
<xml_diff>
--- a/docs/Extra/ActiPASS-Diary-example.xlsx
+++ b/docs/Extra/ActiPASS-Diary-example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pashe866\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pashe866\Coding\Matlab\AMM\Ergo-Tools\ActiPASS\docs\Extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -590,7 +590,7 @@
   <dimension ref="A1:F159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -847,10 +847,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>1000002</v>
+        <v>1000001</v>
       </c>
       <c r="B18" s="1">
-        <v>42898</v>
+        <v>42900</v>
       </c>
       <c r="C18" s="2">
         <v>0.3125</v>
@@ -861,10 +861,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>1000002</v>
+        <v>1000001</v>
       </c>
       <c r="B19" s="1">
-        <v>42898</v>
+        <v>42900</v>
       </c>
       <c r="C19" s="2">
         <v>0.60416666666666663</v>
@@ -878,7 +878,7 @@
         <v>1000001</v>
       </c>
       <c r="B20" s="1">
-        <v>42893</v>
+        <v>42900</v>
       </c>
       <c r="C20" s="2">
         <v>0.85416666666666663</v>

</xml_diff>

<commit_message>
Fixed minor problems in ActiPASS example diary
</commit_message>
<xml_diff>
--- a/docs/Extra/ActiPASS-Diary-example.xlsx
+++ b/docs/Extra/ActiPASS-Diary-example.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pashe866\Coding\Matlab\AMM\Ergo-Tools\ActiPASS\docs\Extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A61346-FE24-4621-879B-D8C3FEEB22F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12330"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExampleData" sheetId="1" r:id="rId1"/>
@@ -25,13 +26,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Pasan Hettiarachchi</author>
     <author>Peter Palm</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -55,7 +56,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="1" shapeId="0">
+    <comment ref="D3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -80,7 +81,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D6" authorId="1" shapeId="0">
+    <comment ref="D6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -109,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="66">
   <si>
     <t>ID</t>
   </si>
@@ -147,9 +148,6 @@
     <t>Stop</t>
   </si>
   <si>
-    <t>ref</t>
-  </si>
-  <si>
     <t xml:space="preserve">Date and time </t>
   </si>
   <si>
@@ -207,9 +205,6 @@
     <t>The 'MNW' is a not-worn period and all activities detected in this period will ignored and will be be re-classified as NW. Can be used in special situations like accelerometer is carried in a bag, but not-worn</t>
   </si>
   <si>
-    <t xml:space="preserve">The event name "Ref" can be used if a reference position (Standing still upright) has been used to adjust the inclination angle of the accelerometer.  </t>
-  </si>
-  <si>
     <t>The even name 'NE' represents 'no event' in ActiPASS terminology. It can be used to end an event where the next event is unknown. Anyway ths is not a special event, but just a suggested naming convention</t>
   </si>
   <si>
@@ -255,9 +250,6 @@
     <t>08:25:00</t>
   </si>
   <si>
-    <t>08:27:00</t>
-  </si>
-  <si>
     <t>16:30:00</t>
   </si>
   <si>
@@ -298,12 +290,30 @@
   </si>
   <si>
     <t>15:30:00</t>
+  </si>
+  <si>
+    <t>08:30:00</t>
+  </si>
+  <si>
+    <t>08:27:42</t>
+  </si>
+  <si>
+    <t>standing still for individual calibration</t>
+  </si>
+  <si>
+    <t>06:30:00</t>
+  </si>
+  <si>
+    <t>06:27:45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The event name "Ref" can be used if a reference position (Standing still upright) is used for individual calibration.  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -425,6 +435,11 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
@@ -512,6 +527,11 @@
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
@@ -854,10 +874,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F159"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F160"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -884,13 +906,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>10</v>
@@ -898,27 +920,30 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>3</v>
@@ -926,13 +951,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>4</v>
@@ -940,13 +965,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>9</v>
@@ -954,13 +979,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>4</v>
@@ -968,13 +993,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>3</v>
@@ -982,13 +1007,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>4</v>
@@ -996,30 +1021,30 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>4</v>
@@ -1027,13 +1052,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>9</v>
@@ -1041,13 +1066,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>4</v>
@@ -1055,13 +1080,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>3</v>
@@ -1069,13 +1094,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>4</v>
@@ -1083,13 +1108,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>3</v>
@@ -1097,30 +1122,30 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>3</v>
@@ -1128,13 +1153,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>4</v>
@@ -1142,13 +1167,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>11</v>
@@ -1156,13 +1181,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>10</v>
@@ -1170,247 +1195,258 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B24" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="D24" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>49</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B28" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>53</v>
-      </c>
       <c r="D28" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E28" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>4</v>
+        <v>29</v>
+      </c>
+      <c r="E29" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D38" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D39" s="1"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D40" s="1"/>
@@ -1437,8 +1473,7 @@
       <c r="D47" s="1"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C48" s="7"/>
-      <c r="D48" s="3"/>
+      <c r="D48" s="1"/>
     </row>
     <row r="49" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C49" s="7"/>
@@ -1473,11 +1508,11 @@
       <c r="D56" s="3"/>
     </row>
     <row r="57" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D57" s="1"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="3"/>
     </row>
     <row r="58" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D58" s="1"/>
-      <c r="F58" s="2"/>
     </row>
     <row r="59" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D59" s="1"/>
@@ -1485,6 +1520,7 @@
     </row>
     <row r="60" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D60" s="1"/>
+      <c r="F60" s="2"/>
     </row>
     <row r="61" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D61" s="1"/>
@@ -1672,10 +1708,10 @@
     <row r="122" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D122" s="1"/>
     </row>
-    <row r="123" spans="4:4" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D123" s="1"/>
     </row>
-    <row r="124" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="4:4" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D124" s="1"/>
     </row>
     <row r="125" spans="4:4" x14ac:dyDescent="0.25">
@@ -1782,6 +1818,9 @@
     </row>
     <row r="159" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D159" s="1"/>
+    </row>
+    <row r="160" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D160" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1792,10 +1831,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1811,23 +1852,23 @@
     <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1835,12 +1876,12 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9"/>
       <c r="D9"/>
@@ -1848,57 +1889,57 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" t="s">
         <v>30</v>
-      </c>
-      <c r="B19" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1906,7 +1947,7 @@
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1916,7 +1957,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor edits to ActiPASS example diary
</commit_message>
<xml_diff>
--- a/docs/Extra/ActiPASS-Diary-example.xlsx
+++ b/docs/Extra/ActiPASS-Diary-example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pashe866\Coding\Matlab\AMM\Ergo-Tools\ActiPASS\docs\Extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A61346-FE24-4621-879B-D8C3FEEB22F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F202A7F-BC56-44F8-A1B7-AC1BF613F0A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExampleData" sheetId="1" r:id="rId1"/>
@@ -877,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F160"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1834,7 +1834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>

</xml_diff>